<commit_message>
Modified Create workflow plan
</commit_message>
<xml_diff>
--- a/Patient Basic Information.xlsx
+++ b/Patient Basic Information.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Testcomplete\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D967C2BB-CEF3-4AAF-8E7E-6CFFCDB83268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA00BB33-4494-4E88-903A-24B99C0199D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FE9CF04E-3282-4EA9-8C0F-537E35FA556C}"/>
   </bookViews>
@@ -284,7 +284,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipertaut" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -301,7 +301,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -619,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D781A32-1DB3-4F4F-87EE-51668E9CA40C}">
   <dimension ref="A1:AC3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T16" sqref="T16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,46 +743,46 @@
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>100000226614</v>
+        <v>100000226615</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="G2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="H2" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="I2" t="s">
         <v>33</v>
       </c>
       <c r="J2" s="1">
-        <v>24662</v>
+        <v>37683</v>
       </c>
       <c r="K2">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="L2">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="M2" t="s">
         <v>34</v>
       </c>
       <c r="N2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O2" t="s">
         <v>37</v>
@@ -791,31 +791,31 @@
         <v>37</v>
       </c>
       <c r="Q2" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="R2" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="S2" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="T2">
-        <v>12170</v>
+        <v>12110</v>
       </c>
       <c r="U2" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="V2" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="W2" t="s">
         <v>41</v>
       </c>
-      <c r="X2" t="s">
-        <v>42</v>
+      <c r="X2" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="Y2" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="Z2" t="s">
         <v>44</v>
@@ -832,46 +832,46 @@
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>100000226615</v>
+        <v>100000226614</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
         <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="G3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="H3" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="I3" t="s">
         <v>33</v>
       </c>
       <c r="J3" s="1">
-        <v>37683</v>
+        <v>24662</v>
       </c>
       <c r="K3">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="L3">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="M3" t="s">
         <v>34</v>
       </c>
       <c r="N3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O3" t="s">
         <v>37</v>
@@ -880,31 +880,31 @@
         <v>37</v>
       </c>
       <c r="Q3" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="R3" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="S3" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="T3">
-        <v>12110</v>
+        <v>12170</v>
       </c>
       <c r="U3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="V3" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="W3" t="s">
         <v>41</v>
       </c>
-      <c r="X3" s="2" t="s">
-        <v>62</v>
+      <c r="X3" t="s">
+        <v>42</v>
       </c>
       <c r="Y3" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="Z3" t="s">
         <v>44</v>
@@ -922,7 +922,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="X3" r:id="rId1" xr:uid="{C605745F-CE93-47B9-8128-37BCC4145BA3}"/>
+    <hyperlink ref="X2" r:id="rId1" xr:uid="{C605745F-CE93-47B9-8128-37BCC4145BA3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>